<commit_message>
cambio al cascada 211/ limpieza
</commit_message>
<xml_diff>
--- a/Tablas/Tabla2bc.xlsx
+++ b/Tablas/Tabla2bc.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="2orSC" sheetId="1" r:id="rId1"/>
-    <sheet name="2-1Cascade" sheetId="4" r:id="rId2"/>
-    <sheet name="2orGM" sheetId="3" r:id="rId3"/>
+    <sheet name="2-1-1" sheetId="6" r:id="rId1"/>
+    <sheet name="2orSC" sheetId="1" r:id="rId2"/>
+    <sheet name="2-1Cascade" sheetId="4" r:id="rId3"/>
+    <sheet name="2orGM" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
   <si>
     <t>Min</t>
   </si>
@@ -105,6 +106,39 @@
   </si>
   <si>
     <t>lin</t>
+  </si>
+  <si>
+    <t>Adc3</t>
+  </si>
+  <si>
+    <t>Adc4</t>
+  </si>
+  <si>
+    <t>gm1(A/V)</t>
+  </si>
+  <si>
+    <t>io1(A)</t>
+  </si>
+  <si>
+    <t>gm2(A/V)</t>
+  </si>
+  <si>
+    <t>io2(A)</t>
+  </si>
+  <si>
+    <t>gm3(A/V)</t>
+  </si>
+  <si>
+    <t>io3(A)</t>
+  </si>
+  <si>
+    <t>gm4(A/V)</t>
+  </si>
+  <si>
+    <t>io4(A)</t>
+  </si>
+  <si>
+    <t>Este modulador proporciona valores de SNR muy altos por lo que no se filtro ninguno (ya que el criterio era SNR&lt;50)</t>
   </si>
 </sst>
 </file>
@@ -186,13 +220,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,6 +507,249 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="7"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G2" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J2" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="5">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M2" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I3" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="L3" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="P3" s="1">
+        <v>50000</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>19720</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="1">
+        <f>(1-Q3/P3)*100</f>
+        <v>60.56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F12" s="6"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F15" s="3"/>
+      <c r="H15" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="P1:Q1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -500,10 +777,10 @@
       <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -616,7 +893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -651,10 +928,10 @@
       <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -795,11 +1072,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -838,10 +1115,10 @@
       <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="3"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -882,7 +1159,7 @@
       <c r="B3" s="1">
         <v>1000</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>1000</v>
       </c>
       <c r="D3" s="1">
@@ -891,7 +1168,7 @@
       <c r="E3" s="1">
         <v>1000</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>1000</v>
       </c>
       <c r="G3" s="1">
@@ -980,11 +1257,11 @@
       <c r="H6" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F13" s="7"/>
+      <c r="F13" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F16" s="4"/>
-      <c r="H16" s="5"/>
+      <c r="F16" s="3"/>
+      <c r="H16" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>